<commit_message>
updated one zip file
</commit_message>
<xml_diff>
--- a/coordinate_output.xlsx
+++ b/coordinate_output.xlsx
@@ -471,12 +471,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>lat</t>
+          <t>latitude</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>lng</t>
+          <t>longitude</t>
         </is>
       </c>
     </row>
@@ -512,15 +512,11 @@
           <t>District of Columbia</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>38.9025154</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>-77.0096286</t>
-        </is>
+      <c r="H2" t="n">
+        <v>38.9025154</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-77.0096286</v>
       </c>
     </row>
     <row r="3">
@@ -555,15 +551,11 @@
           <t>New Castle</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>39.8192755</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>-75.5493308</t>
-        </is>
+      <c r="H3" t="n">
+        <v>39.8192755</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-75.54933080000001</v>
       </c>
     </row>
     <row r="4">
@@ -598,15 +590,11 @@
           <t>Kent</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>39.171610492644476</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>-75.51992693338828</t>
-        </is>
+      <c r="H4" t="n">
+        <v>39.1716105</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-75.5199269</v>
       </c>
     </row>
     <row r="5">
@@ -645,15 +633,11 @@
           <t>New London</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>41.37608734538968</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>-72.14288509703742</t>
-        </is>
+      <c r="H5" t="n">
+        <v>41.3760873</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-72.1428851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>